<commit_message>
editing tasks is possible now
</commit_message>
<xml_diff>
--- a/Documentation/Time Management/Zeitaufzeichnung_Isabella.xlsx
+++ b/Documentation/Time Management/Zeitaufzeichnung_Isabella.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabellaschmut/Desktop/g2t2/Documentation/Time Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33788DB2-7D2E-CA46-9DA4-F2D99A315136}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190039E0-70FD-3045-99B9-F92708A40D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
     <sheet name="Tätigkeiten" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>Datum</t>
   </si>
@@ -169,6 +169,27 @@
   </si>
   <si>
     <t>Nachbesserungen Frontend</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Feiertage einbinden</t>
+  </si>
+  <si>
+    <t>Statistiken Start</t>
+  </si>
+  <si>
+    <t>Tägliche und wöchentliche Statistiken User</t>
+  </si>
+  <si>
+    <t>faces message view</t>
+  </si>
+  <si>
+    <t>Requests</t>
+  </si>
+  <si>
+    <t>Edit Tasks</t>
   </si>
 </sst>
 </file>
@@ -580,10 +601,10 @@
   <dimension ref="A1:D1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1099,49 +1120,130 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="8"/>
-      <c r="B37" s="7"/>
-      <c r="D37" s="3"/>
+      <c r="A37" s="8">
+        <v>43955</v>
+      </c>
+      <c r="B37" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7"/>
-      <c r="D38" s="3"/>
+      <c r="A38" s="8">
+        <v>43955</v>
+      </c>
+      <c r="B38" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
-      <c r="D39" s="3"/>
+      <c r="A39" s="8">
+        <v>43955</v>
+      </c>
+      <c r="B39" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7"/>
-      <c r="D40" s="3"/>
+      <c r="A40" s="8">
+        <v>43956</v>
+      </c>
+      <c r="B40" s="7">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="8"/>
-      <c r="B41" s="7"/>
-      <c r="D41" s="3"/>
+      <c r="A41" s="8">
+        <v>43957</v>
+      </c>
+      <c r="B41" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
-      <c r="D42" s="3"/>
+      <c r="A42" s="8">
+        <v>43958</v>
+      </c>
+      <c r="B42" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="8"/>
-      <c r="B43" s="7"/>
-      <c r="D43" s="3"/>
+      <c r="A43" s="8">
+        <v>43961</v>
+      </c>
+      <c r="B43" s="7">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="8"/>
-      <c r="B44" s="7"/>
-      <c r="D44" s="3"/>
+      <c r="A44" s="8">
+        <v>43961</v>
+      </c>
+      <c r="B44" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="8"/>
-      <c r="B45" s="7"/>
-      <c r="D45" s="3"/>
+      <c r="A45" s="8">
+        <v>43962</v>
+      </c>
+      <c r="B45" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="8"/>

</xml_diff>

<commit_message>
update time management and testdrehbuch
</commit_message>
<xml_diff>
--- a/Documentation/Time Management/Zeitaufzeichnung_Isabella.xlsx
+++ b/Documentation/Time Management/Zeitaufzeichnung_Isabella.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabellaschmut/Desktop/g2t2/Documentation/Time Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C53D137-A32C-D54B-875C-226A17939B91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757C556F-C773-9A42-A4B2-AFBDB48E19F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="65">
   <si>
     <t>Datum</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>Filter Funktionen</t>
+  </si>
+  <si>
+    <t>Tests schreiben</t>
+  </si>
+  <si>
+    <t>Teammeeting</t>
   </si>
 </sst>
 </file>
@@ -637,10 +643,10 @@
   <dimension ref="A1:D1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C62" sqref="C62"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1548,14 +1554,32 @@
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="8"/>
-      <c r="B65" s="7"/>
-      <c r="D65" s="3"/>
+      <c r="A65" s="8">
+        <v>44000</v>
+      </c>
+      <c r="B65" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="8"/>
-      <c r="B66" s="7"/>
-      <c r="D66" s="3"/>
+      <c r="A66" s="8">
+        <v>44000</v>
+      </c>
+      <c r="B66" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="8"/>

</xml_diff>